<commit_message>
Update dataset (D47 columns)
</commit_message>
<xml_diff>
--- a/data/Test 1 - All benthics, epifaunal and infaunal.xlsx
+++ b/data/Test 1 - All benthics, epifaunal and infaunal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74497340b98dbc31/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cromanpa/Downloads/tandy2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC5AFB39-0365-470A-9B4A-7E4303E2248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323995E-6BBF-9F4A-9C38-DAAE1F9809FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{728E38EC-1EB2-43C2-A5E0-CAB4F13D8282}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{728E38EC-1EB2-43C2-A5E0-CAB4F13D8282}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,19 +510,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175323F3-4FFF-4A02-81A9-2342A9028627}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.26953125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="11" customWidth="1"/>
-    <col min="5" max="6" width="10.90625" style="12"/>
-    <col min="8" max="8" width="10.90625" style="10"/>
+    <col min="2" max="2" width="14.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="11" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="12"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -536,10 +536,10 @@
         <v>12</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>2</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -554,7 +554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="11">
         <v>11.986771778665048</v>
       </c>
@@ -574,7 +574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="11">
         <v>11.657803910791269</v>
       </c>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="11">
         <v>11.9892033831422</v>
       </c>
@@ -614,7 +614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="11">
         <v>12.061899931092668</v>
       </c>
@@ -634,7 +634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="11">
         <v>12.904270126275607</v>
       </c>
@@ -654,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="11">
         <v>12.434663886031966</v>
       </c>
@@ -674,7 +674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="11">
         <v>12.956126772643065</v>
       </c>
@@ -694,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="11">
         <v>12.842592673901157</v>
       </c>
@@ -714,7 +714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="11">
         <v>12.474757435863131</v>
       </c>
@@ -734,7 +734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="11">
         <v>12.875016000957771</v>
       </c>
@@ -754,7 +754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="11">
         <v>12.858197868432573</v>
       </c>
@@ -774,7 +774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="11">
         <v>13.256689899219781</v>
       </c>
@@ -794,7 +794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="11">
         <v>13.254253717032007</v>
       </c>
@@ -814,7 +814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="11">
         <v>13.231180688846226</v>
       </c>
@@ -834,7 +834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="11">
         <v>13.271260404591885</v>
       </c>
@@ -854,7 +854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="11">
         <v>13.232013483996344</v>
       </c>
@@ -874,7 +874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="11">
         <v>13.204825731222497</v>
       </c>
@@ -894,7 +894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="11">
         <v>13.206572496865569</v>
       </c>
@@ -914,7 +914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="11">
         <v>13.10974206751993</v>
       </c>
@@ -934,7 +934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="11">
         <v>13.278909359303935</v>
       </c>
@@ -954,7 +954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="11">
         <v>12.123251216153699</v>
       </c>
@@ -974,7 +974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="11">
         <v>12.794559980072737</v>
       </c>
@@ -994,7 +994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="11">
         <v>12.918233096749121</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="11">
         <v>12.841196464823035</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="11">
         <v>13.646695814093361</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="11">
         <v>12.038257950627605</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="11">
         <v>11.999878496056272</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="11">
         <v>12.836933917681204</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="11">
         <v>12.922268943668669</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="11">
         <v>12.844867719471047</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="11">
         <v>11.819686835840555</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="11">
         <v>11.813774745235198</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="11">
         <v>12.081083507759484</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="11">
         <v>12.670372033505052</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="11">
         <v>13.319723147445693</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="11">
         <v>13.47993623641336</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="11">
         <v>13.589960370784754</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="11">
         <v>12.566885416796326</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="11">
         <v>13.349466276399664</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="11">
         <v>13.29277353074923</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="11">
         <v>12.094826263977362</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="11">
         <v>13.281102581509685</v>
       </c>
@@ -1403,20 +1403,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273621F3-3857-447E-AA4B-82306B03B706}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <f>A2+1</f>
         <v>2</v>
@@ -1468,7 +1468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A64" si="0">A3+1</f>
         <v>3</v>
@@ -1486,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1504,7 +1504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1522,7 +1522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1540,7 +1540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1576,7 +1576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1594,7 +1594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1612,7 +1612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1630,7 +1630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1648,7 +1648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1666,7 +1666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1684,7 +1684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1702,7 +1702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1720,7 +1720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1738,7 +1738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1756,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1774,7 +1774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1792,7 +1792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1810,7 +1810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1828,7 +1828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1846,7 +1846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1864,7 +1864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1882,7 +1882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1900,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1918,7 +1918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1936,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1954,7 +1954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1972,7 +1972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1990,7 +1990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2008,7 +2008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2026,7 +2026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2044,7 +2044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2062,7 +2062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2080,7 +2080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2098,7 +2098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2116,7 +2116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2134,7 +2134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2152,7 +2152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2170,7 +2170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2188,7 +2188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2206,7 +2206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2224,7 +2224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2242,7 +2242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2260,7 +2260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2278,7 +2278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2296,7 +2296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2314,7 +2314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2332,7 +2332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2350,7 +2350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2368,7 +2368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2386,7 +2386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2404,7 +2404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2422,7 +2422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2440,7 +2440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2458,7 +2458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2476,7 +2476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2494,7 +2494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2512,7 +2512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2530,7 +2530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2548,7 +2548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <f t="shared" si="0"/>
         <v>63</v>

</xml_diff>

<commit_message>
Update reconstructions and parameters
</commit_message>
<xml_diff>
--- a/data/Test 1 - All benthics, epifaunal and infaunal.xlsx
+++ b/data/Test 1 - All benthics, epifaunal and infaunal.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cromanpa/Downloads/tandy2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hantan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323995E-6BBF-9F4A-9C38-DAAE1F9809FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0CEE6D-2E80-F944-8233-D7A1AF3BD070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{728E38EC-1EB2-43C2-A5E0-CAB4F13D8282}"/>
+    <workbookView xWindow="32980" yWindow="500" windowWidth="29000" windowHeight="17680" xr2:uid="{728E38EC-1EB2-43C2-A5E0-CAB4F13D8282}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
     <sheet name="Reconstruction" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,9 +40,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Temperature error</t>
-  </si>
-  <si>
-    <t>D47 error</t>
   </si>
   <si>
     <t>D47</t>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Temperature (10^6/T(K)^2)</t>
+  </si>
+  <si>
+    <t>D47error</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,34 +524,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1418,19 +1418,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>